<commit_message>
corrections create results and IRR calculation
</commit_message>
<xml_diff>
--- a/emlabpy/Yearly_results.xlsx
+++ b/emlabpy/Yearly_results.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -660,6 +660,56 @@
       </c>
       <c r="P4" t="n">
         <v>-153300.2632881147</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C5" t="n">
+        <v>544999999.1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>20811313152.32112</v>
+      </c>
+      <c r="E5" t="n">
+        <v>38.1858957553916</v>
+      </c>
+      <c r="F5" t="n">
+        <v>11</v>
+      </c>
+      <c r="G5" t="n">
+        <v>222307.2994627971</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2.560297453063297</v>
+      </c>
+      <c r="J5" t="n">
+        <v>97504.61057238668</v>
+      </c>
+      <c r="K5" t="n">
+        <v>17769.20341851865</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.1822396224568984</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>711988264.0362152</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -673,7 +723,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BB4"/>
+  <dimension ref="A1:BB5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1437,6 +1487,170 @@
         <v>0</v>
       </c>
       <c r="BB4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4644.4034</v>
+      </c>
+      <c r="D5" t="n">
+        <v>25208582.8382924</v>
+      </c>
+      <c r="E5" t="n">
+        <v>954932128.661841</v>
+      </c>
+      <c r="F5" t="n">
+        <v>37.88123016623044</v>
+      </c>
+      <c r="G5" t="n">
+        <v>24845.77</v>
+      </c>
+      <c r="H5" t="n">
+        <v>59003.61621933627</v>
+      </c>
+      <c r="I5" t="n">
+        <v>3332129.912351787</v>
+      </c>
+      <c r="J5" t="n">
+        <v>56.47331682121212</v>
+      </c>
+      <c r="K5" t="n">
+        <v>31358.329</v>
+      </c>
+      <c r="L5" t="n">
+        <v>217108263.1152519</v>
+      </c>
+      <c r="M5" t="n">
+        <v>8460882562.993628</v>
+      </c>
+      <c r="N5" t="n">
+        <v>38.97079936797324</v>
+      </c>
+      <c r="O5" t="n">
+        <v>8194.3025</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1007081.087896536</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>53413355.2968122</v>
+      </c>
+      <c r="R5" t="n">
+        <v>53.03779004367492</v>
+      </c>
+      <c r="S5" t="n">
+        <v>8858.749999999998</v>
+      </c>
+      <c r="T5" t="n">
+        <v>18624635.99999999</v>
+      </c>
+      <c r="U5" t="n">
+        <v>705091697.2187846</v>
+      </c>
+      <c r="V5" t="n">
+        <v>37.85801221665675</v>
+      </c>
+      <c r="W5" t="n">
+        <v>8599</v>
+      </c>
+      <c r="X5" t="n">
+        <v>74259244.44886312</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>2846665877.166388</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>38.33416160228613</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>47547.50848700004</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>80823362.9723005</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>2945418492.530766</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>36.44266192610929</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>10271.8</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>40873004.28171189</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>1517259559.244995</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>37.12131236518557</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>53555.51607579708</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>50877740.2720072</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>1831210598.874818</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>35.9923728743579</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>20779.02</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>36159080.46745713</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>1493106750.420732</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>41.29271903815462</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>3652.9</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB5" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>